<commit_message>
Fix typo in cog_dataset_1.xlsx
</commit_message>
<xml_diff>
--- a/data/cog_dataset_1.xlsx
+++ b/data/cog_dataset_1.xlsx
@@ -1,22 +1,39 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24326"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu\home\kobifeldman\Code-Complexity-Research\complexity-verification-project\data\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D867B724-7B14-4604-90A2-1EF71C786BFD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="225" yWindow="225" windowWidth="21360" windowHeight="13155" tabRatio="500"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="dataTasks.xlsx" sheetId="1" r:id="rId1"/>
     <sheet name="Tabelle1" sheetId="2" r:id="rId2"/>
     <sheet name="Tabelle2" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1592" uniqueCount="1255">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1592" uniqueCount="1256">
   <si>
     <t>expCode</t>
   </si>
@@ -4128,15 +4145,25 @@
   <si>
     <t>2: completely correct</t>
   </si>
+  <si>
+    <t>8::Correct</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="20">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="21" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Verdana"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
@@ -4627,392 +4654,393 @@
   </borders>
   <cellStyleXfs count="141">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="10" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="11" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="11" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="12" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="10" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="11" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="11" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="12" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="19" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="19" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="19" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="19" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="19" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="19" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="19" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="19" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="19" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="19" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="19" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="19" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="13" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="13" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="13" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="13" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="13" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="13" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="13" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="13" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="13" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="13" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="13" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="13" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="13" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="13" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="13" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="13" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="13" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="13" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="13" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="13" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="13" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="13" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="13" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="13" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="13" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="13" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="13" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="13" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="13" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="13" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="13" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="13" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="13" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="13" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="13" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="13" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="13" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="13" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="13" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="13" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="13" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="13" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="13" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="13" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="13" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="13" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="13" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="13" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="13" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="13" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="93">
+  <cellXfs count="94">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="20" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="20" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="39" borderId="0" xfId="127" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="39" borderId="0" xfId="127" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="38" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="39" borderId="0" xfId="131" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="41" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="47" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="39" borderId="0" xfId="131" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="41" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="47" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="46" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="43" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="63" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="64" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="60" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="56" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="59" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="61" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="53" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="69" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="46" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="43" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="63" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="64" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="60" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="56" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="59" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="61" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="53" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="69" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="71" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="48" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="70" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="80" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="81" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="67" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="42" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="75" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="90" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="91" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="72" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="44" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="85" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="103" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="73" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="96" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="101" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="99" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="83" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="74" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="93" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="57" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="97" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="105" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="107" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="109" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="71" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="48" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="70" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="80" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="81" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="67" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="42" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="75" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="90" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="91" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="72" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="44" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="85" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="103" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="73" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="96" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="101" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="99" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="83" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="74" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="93" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="57" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="97" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="105" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="107" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="109" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="109" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="111" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="113" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="115" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="117" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="119" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="121" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="123" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="125" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="129" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="131" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="133" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="39" borderId="0" xfId="115" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="39" borderId="0" xfId="119" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="39" borderId="0" xfId="123" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="39" borderId="0" xfId="111" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="39" borderId="0" xfId="107" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="39" borderId="0" xfId="97" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="39" borderId="0" xfId="93" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="39" borderId="0" xfId="83" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="39" borderId="0" xfId="101" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="38" borderId="0" xfId="73" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="39" borderId="0" xfId="72" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="39" borderId="0" xfId="85" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="39" borderId="0" xfId="73" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="39" borderId="0" xfId="75" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="39" borderId="0" xfId="67" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="39" borderId="0" xfId="70" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="39" borderId="0" xfId="56" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="39" borderId="0" xfId="61" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="39" borderId="0" xfId="71" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="39" borderId="0" xfId="64" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="39" borderId="0" xfId="43" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="39" borderId="0" xfId="47" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="109" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="111" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="113" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="115" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="117" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="119" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="121" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="123" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="125" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="129" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="131" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="133" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="39" borderId="0" xfId="115" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="39" borderId="0" xfId="119" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="39" borderId="0" xfId="123" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="39" borderId="0" xfId="111" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="39" borderId="0" xfId="107" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="39" borderId="0" xfId="97" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="39" borderId="0" xfId="93" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="39" borderId="0" xfId="83" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="39" borderId="0" xfId="101" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="38" borderId="0" xfId="73" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="39" borderId="0" xfId="72" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="39" borderId="0" xfId="85" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="39" borderId="0" xfId="73" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="39" borderId="0" xfId="75" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="39" borderId="0" xfId="67" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="39" borderId="0" xfId="70" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="39" borderId="0" xfId="56" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="39" borderId="0" xfId="61" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="39" borderId="0" xfId="71" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="39" borderId="0" xfId="64" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="39" borderId="0" xfId="43" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="39" borderId="0" xfId="47" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="63" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="141">
-    <cellStyle name="20% - Akzent1" xfId="18" builtinId="30" customBuiltin="1"/>
-    <cellStyle name="20% - Akzent2" xfId="22" builtinId="34" customBuiltin="1"/>
-    <cellStyle name="20% - Akzent3" xfId="26" builtinId="38" customBuiltin="1"/>
-    <cellStyle name="20% - Akzent4" xfId="30" builtinId="42" customBuiltin="1"/>
-    <cellStyle name="20% - Akzent5" xfId="34" builtinId="46" customBuiltin="1"/>
-    <cellStyle name="20% - Akzent6" xfId="38" builtinId="50" customBuiltin="1"/>
-    <cellStyle name="40% - Akzent1" xfId="19" builtinId="31" customBuiltin="1"/>
-    <cellStyle name="40% - Akzent2" xfId="23" builtinId="35" customBuiltin="1"/>
-    <cellStyle name="40% - Akzent3" xfId="27" builtinId="39" customBuiltin="1"/>
-    <cellStyle name="40% - Akzent4" xfId="31" builtinId="43" customBuiltin="1"/>
-    <cellStyle name="40% - Akzent5" xfId="35" builtinId="47" customBuiltin="1"/>
-    <cellStyle name="40% - Akzent6" xfId="39" builtinId="51" customBuiltin="1"/>
-    <cellStyle name="60% - Akzent1" xfId="20" builtinId="32" customBuiltin="1"/>
-    <cellStyle name="60% - Akzent2" xfId="24" builtinId="36" customBuiltin="1"/>
-    <cellStyle name="60% - Akzent3" xfId="28" builtinId="40" customBuiltin="1"/>
-    <cellStyle name="60% - Akzent4" xfId="32" builtinId="44" customBuiltin="1"/>
-    <cellStyle name="60% - Akzent5" xfId="36" builtinId="48" customBuiltin="1"/>
-    <cellStyle name="60% - Akzent6" xfId="40" builtinId="52" customBuiltin="1"/>
-    <cellStyle name="Akzent1" xfId="17" builtinId="29" customBuiltin="1"/>
-    <cellStyle name="Akzent2" xfId="21" builtinId="33" customBuiltin="1"/>
-    <cellStyle name="Akzent3" xfId="25" builtinId="37" customBuiltin="1"/>
-    <cellStyle name="Akzent4" xfId="29" builtinId="41" customBuiltin="1"/>
-    <cellStyle name="Akzent5" xfId="33" builtinId="45" customBuiltin="1"/>
-    <cellStyle name="Akzent6" xfId="37" builtinId="49" customBuiltin="1"/>
-    <cellStyle name="Ausgabe" xfId="10" builtinId="21" customBuiltin="1"/>
-    <cellStyle name="Berechnung" xfId="11" builtinId="22" customBuiltin="1"/>
-    <cellStyle name="Eingabe" xfId="9" builtinId="20" customBuiltin="1"/>
-    <cellStyle name="Ergebnis" xfId="16" builtinId="25" customBuiltin="1"/>
-    <cellStyle name="Erklärender Text" xfId="15" builtinId="53" customBuiltin="1"/>
-    <cellStyle name="Gut" xfId="6" builtinId="26" customBuiltin="1"/>
+    <cellStyle name="20% - Accent1" xfId="18" builtinId="30" customBuiltin="1"/>
+    <cellStyle name="20% - Accent2" xfId="22" builtinId="34" customBuiltin="1"/>
+    <cellStyle name="20% - Accent3" xfId="26" builtinId="38" customBuiltin="1"/>
+    <cellStyle name="20% - Accent4" xfId="30" builtinId="42" customBuiltin="1"/>
+    <cellStyle name="20% - Accent5" xfId="34" builtinId="46" customBuiltin="1"/>
+    <cellStyle name="20% - Accent6" xfId="38" builtinId="50" customBuiltin="1"/>
+    <cellStyle name="40% - Accent1" xfId="19" builtinId="31" customBuiltin="1"/>
+    <cellStyle name="40% - Accent2" xfId="23" builtinId="35" customBuiltin="1"/>
+    <cellStyle name="40% - Accent3" xfId="27" builtinId="39" customBuiltin="1"/>
+    <cellStyle name="40% - Accent4" xfId="31" builtinId="43" customBuiltin="1"/>
+    <cellStyle name="40% - Accent5" xfId="35" builtinId="47" customBuiltin="1"/>
+    <cellStyle name="40% - Accent6" xfId="39" builtinId="51" customBuiltin="1"/>
+    <cellStyle name="60% - Accent1" xfId="20" builtinId="32" customBuiltin="1"/>
+    <cellStyle name="60% - Accent2" xfId="24" builtinId="36" customBuiltin="1"/>
+    <cellStyle name="60% - Accent3" xfId="28" builtinId="40" customBuiltin="1"/>
+    <cellStyle name="60% - Accent4" xfId="32" builtinId="44" customBuiltin="1"/>
+    <cellStyle name="60% - Accent5" xfId="36" builtinId="48" customBuiltin="1"/>
+    <cellStyle name="60% - Accent6" xfId="40" builtinId="52" customBuiltin="1"/>
+    <cellStyle name="Accent1" xfId="17" builtinId="29" customBuiltin="1"/>
+    <cellStyle name="Accent2" xfId="21" builtinId="33" customBuiltin="1"/>
+    <cellStyle name="Accent3" xfId="25" builtinId="37" customBuiltin="1"/>
+    <cellStyle name="Accent4" xfId="29" builtinId="41" customBuiltin="1"/>
+    <cellStyle name="Accent5" xfId="33" builtinId="45" customBuiltin="1"/>
+    <cellStyle name="Accent6" xfId="37" builtinId="49" customBuiltin="1"/>
+    <cellStyle name="Bad" xfId="7" builtinId="27" customBuiltin="1"/>
+    <cellStyle name="Calculation" xfId="11" builtinId="22" customBuiltin="1"/>
+    <cellStyle name="Check Cell" xfId="13" builtinId="23" customBuiltin="1"/>
+    <cellStyle name="Explanatory Text" xfId="15" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="Good" xfId="6" builtinId="26" customBuiltin="1"/>
+    <cellStyle name="Heading 1" xfId="2" builtinId="16" customBuiltin="1"/>
+    <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
+    <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
+    <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
+    <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
     <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
-    <cellStyle name="Notiz 10" xfId="50"/>
-    <cellStyle name="Notiz 11" xfId="66"/>
-    <cellStyle name="Notiz 12" xfId="68"/>
-    <cellStyle name="Notiz 13" xfId="58"/>
-    <cellStyle name="Notiz 14" xfId="77"/>
-    <cellStyle name="Notiz 15" xfId="78"/>
-    <cellStyle name="Notiz 16" xfId="82"/>
-    <cellStyle name="Notiz 17" xfId="79"/>
-    <cellStyle name="Notiz 18" xfId="76"/>
-    <cellStyle name="Notiz 19" xfId="87"/>
-    <cellStyle name="Notiz 2" xfId="49"/>
-    <cellStyle name="Notiz 20" xfId="88"/>
-    <cellStyle name="Notiz 21" xfId="92"/>
-    <cellStyle name="Notiz 22" xfId="89"/>
-    <cellStyle name="Notiz 23" xfId="86"/>
-    <cellStyle name="Notiz 24" xfId="98"/>
-    <cellStyle name="Notiz 25" xfId="100"/>
-    <cellStyle name="Notiz 26" xfId="104"/>
-    <cellStyle name="Notiz 27" xfId="102"/>
-    <cellStyle name="Notiz 28" xfId="95"/>
-    <cellStyle name="Notiz 29" xfId="94"/>
-    <cellStyle name="Notiz 3" xfId="45"/>
-    <cellStyle name="Notiz 30" xfId="84"/>
-    <cellStyle name="Notiz 31" xfId="106"/>
-    <cellStyle name="Notiz 32" xfId="108"/>
-    <cellStyle name="Notiz 33" xfId="110"/>
-    <cellStyle name="Notiz 34" xfId="112"/>
-    <cellStyle name="Notiz 35" xfId="114"/>
-    <cellStyle name="Notiz 36" xfId="116"/>
-    <cellStyle name="Notiz 37" xfId="118"/>
-    <cellStyle name="Notiz 38" xfId="120"/>
-    <cellStyle name="Notiz 39" xfId="122"/>
-    <cellStyle name="Notiz 4" xfId="52"/>
-    <cellStyle name="Notiz 40" xfId="124"/>
-    <cellStyle name="Notiz 41" xfId="126"/>
-    <cellStyle name="Notiz 42" xfId="128"/>
-    <cellStyle name="Notiz 43" xfId="130"/>
-    <cellStyle name="Notiz 44" xfId="132"/>
-    <cellStyle name="Notiz 45" xfId="134"/>
-    <cellStyle name="Notiz 46" xfId="135"/>
-    <cellStyle name="Notiz 47" xfId="136"/>
-    <cellStyle name="Notiz 48" xfId="137"/>
-    <cellStyle name="Notiz 49" xfId="138"/>
-    <cellStyle name="Notiz 5" xfId="54"/>
-    <cellStyle name="Notiz 50" xfId="139"/>
-    <cellStyle name="Notiz 51" xfId="140"/>
-    <cellStyle name="Notiz 6" xfId="65"/>
-    <cellStyle name="Notiz 7" xfId="55"/>
-    <cellStyle name="Notiz 8" xfId="62"/>
-    <cellStyle name="Notiz 9" xfId="51"/>
-    <cellStyle name="Schlecht" xfId="7" builtinId="27" customBuiltin="1"/>
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
-    <cellStyle name="Standard 10" xfId="59"/>
-    <cellStyle name="Standard 11" xfId="61"/>
-    <cellStyle name="Standard 12" xfId="53"/>
-    <cellStyle name="Standard 13" xfId="69"/>
-    <cellStyle name="Standard 14" xfId="71"/>
-    <cellStyle name="Standard 15" xfId="48"/>
-    <cellStyle name="Standard 16" xfId="70"/>
-    <cellStyle name="Standard 17" xfId="80"/>
-    <cellStyle name="Standard 18" xfId="81"/>
-    <cellStyle name="Standard 19" xfId="67"/>
-    <cellStyle name="Standard 2" xfId="41"/>
-    <cellStyle name="Standard 20" xfId="42"/>
-    <cellStyle name="Standard 21" xfId="75"/>
-    <cellStyle name="Standard 22" xfId="90"/>
-    <cellStyle name="Standard 23" xfId="91"/>
-    <cellStyle name="Standard 24" xfId="72"/>
-    <cellStyle name="Standard 25" xfId="44"/>
-    <cellStyle name="Standard 26" xfId="85"/>
-    <cellStyle name="Standard 27" xfId="103"/>
-    <cellStyle name="Standard 28" xfId="73"/>
-    <cellStyle name="Standard 29" xfId="96"/>
-    <cellStyle name="Standard 3" xfId="47"/>
-    <cellStyle name="Standard 30" xfId="101"/>
-    <cellStyle name="Standard 31" xfId="99"/>
-    <cellStyle name="Standard 32" xfId="83"/>
-    <cellStyle name="Standard 33" xfId="74"/>
-    <cellStyle name="Standard 34" xfId="93"/>
-    <cellStyle name="Standard 35" xfId="57"/>
-    <cellStyle name="Standard 36" xfId="97"/>
-    <cellStyle name="Standard 37" xfId="105"/>
-    <cellStyle name="Standard 38" xfId="107"/>
-    <cellStyle name="Standard 39" xfId="109"/>
-    <cellStyle name="Standard 4" xfId="46"/>
-    <cellStyle name="Standard 40" xfId="111"/>
-    <cellStyle name="Standard 41" xfId="113"/>
-    <cellStyle name="Standard 42" xfId="115"/>
-    <cellStyle name="Standard 43" xfId="117"/>
-    <cellStyle name="Standard 44" xfId="119"/>
-    <cellStyle name="Standard 45" xfId="121"/>
-    <cellStyle name="Standard 46" xfId="123"/>
-    <cellStyle name="Standard 47" xfId="125"/>
-    <cellStyle name="Standard 48" xfId="127"/>
-    <cellStyle name="Standard 49" xfId="129"/>
-    <cellStyle name="Standard 5" xfId="43"/>
-    <cellStyle name="Standard 50" xfId="131"/>
-    <cellStyle name="Standard 51" xfId="133"/>
-    <cellStyle name="Standard 6" xfId="63"/>
-    <cellStyle name="Standard 7" xfId="64"/>
-    <cellStyle name="Standard 8" xfId="60"/>
-    <cellStyle name="Standard 9" xfId="56"/>
-    <cellStyle name="Überschrift" xfId="1" builtinId="15" customBuiltin="1"/>
-    <cellStyle name="Überschrift 1" xfId="2" builtinId="16" customBuiltin="1"/>
-    <cellStyle name="Überschrift 2" xfId="3" builtinId="17" customBuiltin="1"/>
-    <cellStyle name="Überschrift 3" xfId="4" builtinId="18" customBuiltin="1"/>
-    <cellStyle name="Überschrift 4" xfId="5" builtinId="19" customBuiltin="1"/>
-    <cellStyle name="Verknüpfte Zelle" xfId="12" builtinId="24" customBuiltin="1"/>
-    <cellStyle name="Warnender Text" xfId="14" builtinId="11" customBuiltin="1"/>
-    <cellStyle name="Zelle überprüfen" xfId="13" builtinId="23" customBuiltin="1"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Notiz 10" xfId="50" xr:uid="{00000000-0005-0000-0000-00001F000000}"/>
+    <cellStyle name="Notiz 11" xfId="66" xr:uid="{00000000-0005-0000-0000-000020000000}"/>
+    <cellStyle name="Notiz 12" xfId="68" xr:uid="{00000000-0005-0000-0000-000021000000}"/>
+    <cellStyle name="Notiz 13" xfId="58" xr:uid="{00000000-0005-0000-0000-000022000000}"/>
+    <cellStyle name="Notiz 14" xfId="77" xr:uid="{00000000-0005-0000-0000-000023000000}"/>
+    <cellStyle name="Notiz 15" xfId="78" xr:uid="{00000000-0005-0000-0000-000024000000}"/>
+    <cellStyle name="Notiz 16" xfId="82" xr:uid="{00000000-0005-0000-0000-000025000000}"/>
+    <cellStyle name="Notiz 17" xfId="79" xr:uid="{00000000-0005-0000-0000-000026000000}"/>
+    <cellStyle name="Notiz 18" xfId="76" xr:uid="{00000000-0005-0000-0000-000027000000}"/>
+    <cellStyle name="Notiz 19" xfId="87" xr:uid="{00000000-0005-0000-0000-000028000000}"/>
+    <cellStyle name="Notiz 2" xfId="49" xr:uid="{00000000-0005-0000-0000-000029000000}"/>
+    <cellStyle name="Notiz 20" xfId="88" xr:uid="{00000000-0005-0000-0000-00002A000000}"/>
+    <cellStyle name="Notiz 21" xfId="92" xr:uid="{00000000-0005-0000-0000-00002B000000}"/>
+    <cellStyle name="Notiz 22" xfId="89" xr:uid="{00000000-0005-0000-0000-00002C000000}"/>
+    <cellStyle name="Notiz 23" xfId="86" xr:uid="{00000000-0005-0000-0000-00002D000000}"/>
+    <cellStyle name="Notiz 24" xfId="98" xr:uid="{00000000-0005-0000-0000-00002E000000}"/>
+    <cellStyle name="Notiz 25" xfId="100" xr:uid="{00000000-0005-0000-0000-00002F000000}"/>
+    <cellStyle name="Notiz 26" xfId="104" xr:uid="{00000000-0005-0000-0000-000030000000}"/>
+    <cellStyle name="Notiz 27" xfId="102" xr:uid="{00000000-0005-0000-0000-000031000000}"/>
+    <cellStyle name="Notiz 28" xfId="95" xr:uid="{00000000-0005-0000-0000-000032000000}"/>
+    <cellStyle name="Notiz 29" xfId="94" xr:uid="{00000000-0005-0000-0000-000033000000}"/>
+    <cellStyle name="Notiz 3" xfId="45" xr:uid="{00000000-0005-0000-0000-000034000000}"/>
+    <cellStyle name="Notiz 30" xfId="84" xr:uid="{00000000-0005-0000-0000-000035000000}"/>
+    <cellStyle name="Notiz 31" xfId="106" xr:uid="{00000000-0005-0000-0000-000036000000}"/>
+    <cellStyle name="Notiz 32" xfId="108" xr:uid="{00000000-0005-0000-0000-000037000000}"/>
+    <cellStyle name="Notiz 33" xfId="110" xr:uid="{00000000-0005-0000-0000-000038000000}"/>
+    <cellStyle name="Notiz 34" xfId="112" xr:uid="{00000000-0005-0000-0000-000039000000}"/>
+    <cellStyle name="Notiz 35" xfId="114" xr:uid="{00000000-0005-0000-0000-00003A000000}"/>
+    <cellStyle name="Notiz 36" xfId="116" xr:uid="{00000000-0005-0000-0000-00003B000000}"/>
+    <cellStyle name="Notiz 37" xfId="118" xr:uid="{00000000-0005-0000-0000-00003C000000}"/>
+    <cellStyle name="Notiz 38" xfId="120" xr:uid="{00000000-0005-0000-0000-00003D000000}"/>
+    <cellStyle name="Notiz 39" xfId="122" xr:uid="{00000000-0005-0000-0000-00003E000000}"/>
+    <cellStyle name="Notiz 4" xfId="52" xr:uid="{00000000-0005-0000-0000-00003F000000}"/>
+    <cellStyle name="Notiz 40" xfId="124" xr:uid="{00000000-0005-0000-0000-000040000000}"/>
+    <cellStyle name="Notiz 41" xfId="126" xr:uid="{00000000-0005-0000-0000-000041000000}"/>
+    <cellStyle name="Notiz 42" xfId="128" xr:uid="{00000000-0005-0000-0000-000042000000}"/>
+    <cellStyle name="Notiz 43" xfId="130" xr:uid="{00000000-0005-0000-0000-000043000000}"/>
+    <cellStyle name="Notiz 44" xfId="132" xr:uid="{00000000-0005-0000-0000-000044000000}"/>
+    <cellStyle name="Notiz 45" xfId="134" xr:uid="{00000000-0005-0000-0000-000045000000}"/>
+    <cellStyle name="Notiz 46" xfId="135" xr:uid="{00000000-0005-0000-0000-000046000000}"/>
+    <cellStyle name="Notiz 47" xfId="136" xr:uid="{00000000-0005-0000-0000-000047000000}"/>
+    <cellStyle name="Notiz 48" xfId="137" xr:uid="{00000000-0005-0000-0000-000048000000}"/>
+    <cellStyle name="Notiz 49" xfId="138" xr:uid="{00000000-0005-0000-0000-000049000000}"/>
+    <cellStyle name="Notiz 5" xfId="54" xr:uid="{00000000-0005-0000-0000-00004A000000}"/>
+    <cellStyle name="Notiz 50" xfId="139" xr:uid="{00000000-0005-0000-0000-00004B000000}"/>
+    <cellStyle name="Notiz 51" xfId="140" xr:uid="{00000000-0005-0000-0000-00004C000000}"/>
+    <cellStyle name="Notiz 6" xfId="65" xr:uid="{00000000-0005-0000-0000-00004D000000}"/>
+    <cellStyle name="Notiz 7" xfId="55" xr:uid="{00000000-0005-0000-0000-00004E000000}"/>
+    <cellStyle name="Notiz 8" xfId="62" xr:uid="{00000000-0005-0000-0000-00004F000000}"/>
+    <cellStyle name="Notiz 9" xfId="51" xr:uid="{00000000-0005-0000-0000-000050000000}"/>
+    <cellStyle name="Output" xfId="10" builtinId="21" customBuiltin="1"/>
+    <cellStyle name="Standard 10" xfId="59" xr:uid="{00000000-0005-0000-0000-000053000000}"/>
+    <cellStyle name="Standard 11" xfId="61" xr:uid="{00000000-0005-0000-0000-000054000000}"/>
+    <cellStyle name="Standard 12" xfId="53" xr:uid="{00000000-0005-0000-0000-000055000000}"/>
+    <cellStyle name="Standard 13" xfId="69" xr:uid="{00000000-0005-0000-0000-000056000000}"/>
+    <cellStyle name="Standard 14" xfId="71" xr:uid="{00000000-0005-0000-0000-000057000000}"/>
+    <cellStyle name="Standard 15" xfId="48" xr:uid="{00000000-0005-0000-0000-000058000000}"/>
+    <cellStyle name="Standard 16" xfId="70" xr:uid="{00000000-0005-0000-0000-000059000000}"/>
+    <cellStyle name="Standard 17" xfId="80" xr:uid="{00000000-0005-0000-0000-00005A000000}"/>
+    <cellStyle name="Standard 18" xfId="81" xr:uid="{00000000-0005-0000-0000-00005B000000}"/>
+    <cellStyle name="Standard 19" xfId="67" xr:uid="{00000000-0005-0000-0000-00005C000000}"/>
+    <cellStyle name="Standard 2" xfId="41" xr:uid="{00000000-0005-0000-0000-00005D000000}"/>
+    <cellStyle name="Standard 20" xfId="42" xr:uid="{00000000-0005-0000-0000-00005E000000}"/>
+    <cellStyle name="Standard 21" xfId="75" xr:uid="{00000000-0005-0000-0000-00005F000000}"/>
+    <cellStyle name="Standard 22" xfId="90" xr:uid="{00000000-0005-0000-0000-000060000000}"/>
+    <cellStyle name="Standard 23" xfId="91" xr:uid="{00000000-0005-0000-0000-000061000000}"/>
+    <cellStyle name="Standard 24" xfId="72" xr:uid="{00000000-0005-0000-0000-000062000000}"/>
+    <cellStyle name="Standard 25" xfId="44" xr:uid="{00000000-0005-0000-0000-000063000000}"/>
+    <cellStyle name="Standard 26" xfId="85" xr:uid="{00000000-0005-0000-0000-000064000000}"/>
+    <cellStyle name="Standard 27" xfId="103" xr:uid="{00000000-0005-0000-0000-000065000000}"/>
+    <cellStyle name="Standard 28" xfId="73" xr:uid="{00000000-0005-0000-0000-000066000000}"/>
+    <cellStyle name="Standard 29" xfId="96" xr:uid="{00000000-0005-0000-0000-000067000000}"/>
+    <cellStyle name="Standard 3" xfId="47" xr:uid="{00000000-0005-0000-0000-000068000000}"/>
+    <cellStyle name="Standard 30" xfId="101" xr:uid="{00000000-0005-0000-0000-000069000000}"/>
+    <cellStyle name="Standard 31" xfId="99" xr:uid="{00000000-0005-0000-0000-00006A000000}"/>
+    <cellStyle name="Standard 32" xfId="83" xr:uid="{00000000-0005-0000-0000-00006B000000}"/>
+    <cellStyle name="Standard 33" xfId="74" xr:uid="{00000000-0005-0000-0000-00006C000000}"/>
+    <cellStyle name="Standard 34" xfId="93" xr:uid="{00000000-0005-0000-0000-00006D000000}"/>
+    <cellStyle name="Standard 35" xfId="57" xr:uid="{00000000-0005-0000-0000-00006E000000}"/>
+    <cellStyle name="Standard 36" xfId="97" xr:uid="{00000000-0005-0000-0000-00006F000000}"/>
+    <cellStyle name="Standard 37" xfId="105" xr:uid="{00000000-0005-0000-0000-000070000000}"/>
+    <cellStyle name="Standard 38" xfId="107" xr:uid="{00000000-0005-0000-0000-000071000000}"/>
+    <cellStyle name="Standard 39" xfId="109" xr:uid="{00000000-0005-0000-0000-000072000000}"/>
+    <cellStyle name="Standard 4" xfId="46" xr:uid="{00000000-0005-0000-0000-000073000000}"/>
+    <cellStyle name="Standard 40" xfId="111" xr:uid="{00000000-0005-0000-0000-000074000000}"/>
+    <cellStyle name="Standard 41" xfId="113" xr:uid="{00000000-0005-0000-0000-000075000000}"/>
+    <cellStyle name="Standard 42" xfId="115" xr:uid="{00000000-0005-0000-0000-000076000000}"/>
+    <cellStyle name="Standard 43" xfId="117" xr:uid="{00000000-0005-0000-0000-000077000000}"/>
+    <cellStyle name="Standard 44" xfId="119" xr:uid="{00000000-0005-0000-0000-000078000000}"/>
+    <cellStyle name="Standard 45" xfId="121" xr:uid="{00000000-0005-0000-0000-000079000000}"/>
+    <cellStyle name="Standard 46" xfId="123" xr:uid="{00000000-0005-0000-0000-00007A000000}"/>
+    <cellStyle name="Standard 47" xfId="125" xr:uid="{00000000-0005-0000-0000-00007B000000}"/>
+    <cellStyle name="Standard 48" xfId="127" xr:uid="{00000000-0005-0000-0000-00007C000000}"/>
+    <cellStyle name="Standard 49" xfId="129" xr:uid="{00000000-0005-0000-0000-00007D000000}"/>
+    <cellStyle name="Standard 5" xfId="43" xr:uid="{00000000-0005-0000-0000-00007E000000}"/>
+    <cellStyle name="Standard 50" xfId="131" xr:uid="{00000000-0005-0000-0000-00007F000000}"/>
+    <cellStyle name="Standard 51" xfId="133" xr:uid="{00000000-0005-0000-0000-000080000000}"/>
+    <cellStyle name="Standard 6" xfId="63" xr:uid="{00000000-0005-0000-0000-000081000000}"/>
+    <cellStyle name="Standard 7" xfId="64" xr:uid="{00000000-0005-0000-0000-000082000000}"/>
+    <cellStyle name="Standard 8" xfId="60" xr:uid="{00000000-0005-0000-0000-000083000000}"/>
+    <cellStyle name="Standard 9" xfId="56" xr:uid="{00000000-0005-0000-0000-000084000000}"/>
+    <cellStyle name="Title" xfId="1" builtinId="15" customBuiltin="1"/>
+    <cellStyle name="Total" xfId="16" builtinId="25" customBuiltin="1"/>
+    <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -5022,6 +5050,14 @@
       <color rgb="FFFFFF99"/>
     </mruColors>
   </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -5344,16 +5380,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr published="0" enableFormatConditionsCalculation="0"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr published="0"/>
   <dimension ref="A1:EM94"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A38" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C63" sqref="C63"/>
+    <sheetView tabSelected="1" topLeftCell="AN1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="AX1" sqref="AX1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="3" max="4" width="10.75" style="2"/>
     <col min="6" max="6" width="11.875" customWidth="1"/>
@@ -5361,7 +5397,7 @@
     <col min="15" max="16" width="10.75" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:143">
+    <row r="1" spans="1:143" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -5510,7 +5546,7 @@
         <v>1064</v>
       </c>
       <c r="AX1" s="13" t="s">
-        <v>1180</v>
+        <v>1255</v>
       </c>
       <c r="AY1" s="8" t="s">
         <v>1065</v>
@@ -5789,7 +5825,7 @@
         <v>1233</v>
       </c>
     </row>
-    <row r="2" spans="1:143">
+    <row r="2" spans="1:143" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -6215,7 +6251,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="3" spans="1:143">
+    <row r="3" spans="1:143" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -6617,7 +6653,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="4" spans="1:143">
+    <row r="4" spans="1:143" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -7043,7 +7079,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="5" spans="1:143">
+    <row r="5" spans="1:143" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>2</v>
       </c>
@@ -7446,7 +7482,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="6" spans="1:143">
+    <row r="6" spans="1:143" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>2</v>
       </c>
@@ -7872,7 +7908,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="7" spans="1:143">
+    <row r="7" spans="1:143" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>2</v>
       </c>
@@ -8295,7 +8331,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="8" spans="1:143">
+    <row r="8" spans="1:143" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>2</v>
       </c>
@@ -8721,7 +8757,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="9" spans="1:143">
+    <row r="9" spans="1:143" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>2</v>
       </c>
@@ -9144,7 +9180,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="10" spans="1:143">
+    <row r="10" spans="1:143" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>2</v>
       </c>
@@ -9562,7 +9598,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="11" spans="1:143">
+    <row r="11" spans="1:143" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>2</v>
       </c>
@@ -9985,7 +10021,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="12" spans="1:143">
+    <row r="12" spans="1:143" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>2</v>
       </c>
@@ -10411,7 +10447,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="13" spans="1:143">
+    <row r="13" spans="1:143" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>2</v>
       </c>
@@ -10837,7 +10873,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="14" spans="1:143">
+    <row r="14" spans="1:143" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>2</v>
       </c>
@@ -11260,7 +11296,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="15" spans="1:143" ht="12.75" customHeight="1">
+    <row r="15" spans="1:143" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>2</v>
       </c>
@@ -11623,7 +11659,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="16" spans="1:143">
+    <row r="16" spans="1:143" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>2</v>
       </c>
@@ -12037,7 +12073,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="17" spans="1:142">
+    <row r="17" spans="1:142" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>2</v>
       </c>
@@ -12463,7 +12499,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="18" spans="1:142">
+    <row r="18" spans="1:142" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>2</v>
       </c>
@@ -12859,7 +12895,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="19" spans="1:142">
+    <row r="19" spans="1:142" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>2</v>
       </c>
@@ -13274,7 +13310,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="20" spans="1:142">
+    <row r="20" spans="1:142" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>2</v>
       </c>
@@ -13694,7 +13730,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="21" spans="1:142">
+    <row r="21" spans="1:142" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>2</v>
       </c>
@@ -14120,7 +14156,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="22" spans="1:142">
+    <row r="22" spans="1:142" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>2</v>
       </c>
@@ -14546,7 +14582,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="23" spans="1:142" ht="12.75" customHeight="1">
+    <row r="23" spans="1:142" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>2</v>
       </c>
@@ -14972,7 +15008,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="24" spans="1:142">
+    <row r="24" spans="1:142" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>2</v>
       </c>
@@ -15374,7 +15410,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="25" spans="1:142" ht="12.75" customHeight="1">
+    <row r="25" spans="1:142" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>2</v>
       </c>
@@ -15794,7 +15830,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="26" spans="1:142" ht="12.75" customHeight="1">
+    <row r="26" spans="1:142" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>2</v>
       </c>
@@ -16217,7 +16253,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="27" spans="1:142">
+    <row r="27" spans="1:142" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>2</v>
       </c>
@@ -16643,7 +16679,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="28" spans="1:142">
+    <row r="28" spans="1:142" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>2</v>
       </c>
@@ -17045,7 +17081,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="29" spans="1:142">
+    <row r="29" spans="1:142" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>2</v>
       </c>
@@ -17465,7 +17501,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="30" spans="1:142">
+    <row r="30" spans="1:142" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>2</v>
       </c>
@@ -17889,7 +17925,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="31" spans="1:142">
+    <row r="31" spans="1:142" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>2</v>
       </c>
@@ -18309,7 +18345,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="32" spans="1:142">
+    <row r="32" spans="1:142" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>2</v>
       </c>
@@ -18735,7 +18771,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="33" spans="1:142">
+    <row r="33" spans="1:142" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>2</v>
       </c>
@@ -19158,7 +19194,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="34" spans="1:142">
+    <row r="34" spans="1:142" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>2</v>
       </c>
@@ -19581,7 +19617,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="35" spans="1:142">
+    <row r="35" spans="1:142" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>2</v>
       </c>
@@ -20004,7 +20040,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="36" spans="1:142">
+    <row r="36" spans="1:142" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>2</v>
       </c>
@@ -20430,7 +20466,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="37" spans="1:142">
+    <row r="37" spans="1:142" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>2</v>
       </c>
@@ -20856,7 +20892,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="38" spans="1:142">
+    <row r="38" spans="1:142" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>2</v>
       </c>
@@ -21282,7 +21318,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="39" spans="1:142">
+    <row r="39" spans="1:142" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>2</v>
       </c>
@@ -21678,7 +21714,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="40" spans="1:142">
+    <row r="40" spans="1:142" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>2</v>
       </c>
@@ -22104,7 +22140,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="41" spans="1:142">
+    <row r="41" spans="1:142" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>2</v>
       </c>
@@ -22530,7 +22566,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="42" spans="1:142" s="22" customFormat="1" ht="15" customHeight="1">
+    <row r="42" spans="1:142" s="22" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="20" t="s">
         <v>2</v>
       </c>
@@ -22567,7 +22603,7 @@
       <c r="L42" s="24">
         <v>1</v>
       </c>
-      <c r="M42" s="25" t="s">
+      <c r="M42" s="93" t="s">
         <v>1208</v>
       </c>
       <c r="N42" s="25">
@@ -22956,7 +22992,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="44" spans="1:142">
+    <row r="44" spans="1:142" x14ac:dyDescent="0.2">
       <c r="B44" s="10" t="s">
         <v>1140</v>
       </c>
@@ -23237,7 +23273,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="45" spans="1:142">
+    <row r="45" spans="1:142" x14ac:dyDescent="0.2">
       <c r="B45" s="10"/>
       <c r="E45" s="2"/>
       <c r="K45" s="2"/>
@@ -23303,7 +23339,7 @@
       <c r="EF45" s="2"/>
       <c r="EG45" s="2"/>
     </row>
-    <row r="46" spans="1:142">
+    <row r="46" spans="1:142" x14ac:dyDescent="0.2">
       <c r="B46" s="13" t="s">
         <v>1205</v>
       </c>
@@ -23371,7 +23407,7 @@
       <c r="EF46" s="2"/>
       <c r="EG46" s="2"/>
     </row>
-    <row r="47" spans="1:142">
+    <row r="47" spans="1:142" x14ac:dyDescent="0.2">
       <c r="S47" t="s">
         <v>1172</v>
       </c>
@@ -23506,7 +23542,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="48" spans="1:142">
+    <row r="48" spans="1:142" x14ac:dyDescent="0.2">
       <c r="B48" s="10" t="s">
         <v>1142</v>
       </c>
@@ -23659,7 +23695,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="49" spans="2:142">
+    <row r="49" spans="2:142" x14ac:dyDescent="0.2">
       <c r="B49" s="13" t="s">
         <v>1143</v>
       </c>
@@ -23812,7 +23848,7 @@
         <v>36.926829268292686</v>
       </c>
     </row>
-    <row r="50" spans="2:142">
+    <row r="50" spans="2:142" x14ac:dyDescent="0.2">
       <c r="C50" s="6" t="s">
         <v>1241</v>
       </c>
@@ -23836,12 +23872,12 @@
         <v>8.2231084265697199</v>
       </c>
     </row>
-    <row r="51" spans="2:142">
+    <row r="51" spans="2:142" x14ac:dyDescent="0.2">
       <c r="C51" s="6" t="s">
         <v>1242</v>
       </c>
     </row>
-    <row r="52" spans="2:142">
+    <row r="52" spans="2:142" x14ac:dyDescent="0.2">
       <c r="C52" s="6" t="s">
         <v>1243</v>
       </c>
@@ -23849,7 +23885,7 @@
         <v>154.64156097560979</v>
       </c>
     </row>
-    <row r="53" spans="2:142">
+    <row r="53" spans="2:142" x14ac:dyDescent="0.2">
       <c r="F53" t="s">
         <v>1247</v>
       </c>
@@ -23862,7 +23898,7 @@
       <c r="O53"/>
       <c r="P53"/>
     </row>
-    <row r="54" spans="2:142">
+    <row r="54" spans="2:142" x14ac:dyDescent="0.2">
       <c r="B54" s="10" t="s">
         <v>1141</v>
       </c>
@@ -23884,7 +23920,7 @@
       <c r="O54"/>
       <c r="P54"/>
     </row>
-    <row r="55" spans="2:142">
+    <row r="55" spans="2:142" x14ac:dyDescent="0.2">
       <c r="B55" s="10" t="s">
         <v>1144</v>
       </c>
@@ -23906,25 +23942,25 @@
       <c r="O55"/>
       <c r="P55"/>
     </row>
-    <row r="56" spans="2:142">
+    <row r="56" spans="2:142" x14ac:dyDescent="0.2">
       <c r="C56" s="2" t="s">
         <v>1241</v>
       </c>
     </row>
-    <row r="57" spans="2:142">
+    <row r="57" spans="2:142" x14ac:dyDescent="0.2">
       <c r="C57" s="2" t="s">
         <v>1250</v>
       </c>
     </row>
-    <row r="58" spans="2:142">
+    <row r="58" spans="2:142" x14ac:dyDescent="0.2">
       <c r="C58" s="2" t="s">
         <v>1251</v>
       </c>
     </row>
-    <row r="59" spans="2:142">
+    <row r="59" spans="2:142" x14ac:dyDescent="0.2">
       <c r="C59" s="12"/>
     </row>
-    <row r="60" spans="2:142">
+    <row r="60" spans="2:142" x14ac:dyDescent="0.2">
       <c r="B60" t="s">
         <v>1171</v>
       </c>
@@ -23932,137 +23968,137 @@
         <v>1252</v>
       </c>
     </row>
-    <row r="61" spans="2:142">
+    <row r="61" spans="2:142" x14ac:dyDescent="0.2">
       <c r="C61" s="2" t="s">
         <v>1253</v>
       </c>
     </row>
-    <row r="62" spans="2:142">
+    <row r="62" spans="2:142" x14ac:dyDescent="0.2">
       <c r="C62" s="2" t="s">
         <v>1254</v>
       </c>
     </row>
-    <row r="64" spans="2:142">
+    <row r="64" spans="2:142" x14ac:dyDescent="0.2">
       <c r="B64" s="10" t="s">
         <v>1145</v>
       </c>
     </row>
-    <row r="65" spans="3:3">
+    <row r="65" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C65" s="12" t="s">
         <v>1146</v>
       </c>
     </row>
-    <row r="66" spans="3:3">
+    <row r="66" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C66" s="6" t="s">
         <v>1147</v>
       </c>
     </row>
-    <row r="67" spans="3:3">
+    <row r="67" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C67" s="6" t="s">
         <v>1148</v>
       </c>
     </row>
-    <row r="68" spans="3:3">
+    <row r="68" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C68" s="6" t="s">
         <v>1149</v>
       </c>
     </row>
-    <row r="69" spans="3:3">
+    <row r="69" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C69" s="14" t="s">
         <v>1150</v>
       </c>
     </row>
-    <row r="70" spans="3:3">
+    <row r="70" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C70" s="6" t="s">
         <v>1151</v>
       </c>
     </row>
-    <row r="71" spans="3:3">
+    <row r="71" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C71" s="6" t="s">
         <v>1152</v>
       </c>
     </row>
-    <row r="72" spans="3:3">
+    <row r="72" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C72" s="6" t="s">
         <v>1153</v>
       </c>
     </row>
-    <row r="73" spans="3:3">
+    <row r="73" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C73" s="6" t="s">
         <v>1154</v>
       </c>
     </row>
-    <row r="74" spans="3:3">
+    <row r="74" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C74" s="6" t="s">
         <v>1155</v>
       </c>
     </row>
-    <row r="75" spans="3:3">
+    <row r="75" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C75" s="6" t="s">
         <v>1156</v>
       </c>
     </row>
-    <row r="76" spans="3:3">
+    <row r="76" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C76" s="6" t="s">
         <v>1157</v>
       </c>
     </row>
-    <row r="77" spans="3:3">
+    <row r="77" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C77" s="6" t="s">
         <v>1158</v>
       </c>
     </row>
-    <row r="78" spans="3:3">
+    <row r="78" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C78" s="6" t="s">
         <v>1159</v>
       </c>
     </row>
-    <row r="79" spans="3:3">
+    <row r="79" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C79" s="6" t="s">
         <v>1160</v>
       </c>
     </row>
-    <row r="80" spans="3:3">
+    <row r="80" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C80" s="6" t="s">
         <v>1161</v>
       </c>
     </row>
-    <row r="81" spans="2:4">
+    <row r="81" spans="2:4" x14ac:dyDescent="0.2">
       <c r="C81" s="6" t="s">
         <v>1162</v>
       </c>
     </row>
-    <row r="82" spans="2:4">
+    <row r="82" spans="2:4" x14ac:dyDescent="0.2">
       <c r="C82" s="6" t="s">
         <v>1163</v>
       </c>
     </row>
-    <row r="83" spans="2:4">
+    <row r="83" spans="2:4" x14ac:dyDescent="0.2">
       <c r="C83" s="6" t="s">
         <v>1164</v>
       </c>
     </row>
-    <row r="84" spans="2:4">
+    <row r="84" spans="2:4" x14ac:dyDescent="0.2">
       <c r="C84" s="6" t="s">
         <v>1165</v>
       </c>
     </row>
-    <row r="85" spans="2:4">
+    <row r="85" spans="2:4" x14ac:dyDescent="0.2">
       <c r="C85" s="6" t="s">
         <v>1166</v>
       </c>
     </row>
-    <row r="86" spans="2:4">
+    <row r="86" spans="2:4" x14ac:dyDescent="0.2">
       <c r="C86" s="6" t="s">
         <v>1167</v>
       </c>
     </row>
-    <row r="87" spans="2:4">
+    <row r="87" spans="2:4" x14ac:dyDescent="0.2">
       <c r="C87" s="6" t="s">
         <v>1168</v>
       </c>
     </row>
-    <row r="90" spans="2:4">
+    <row r="90" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B90" t="s">
         <v>1199</v>
       </c>
@@ -24070,17 +24106,17 @@
         <v>1204</v>
       </c>
     </row>
-    <row r="91" spans="2:4">
+    <row r="91" spans="2:4" x14ac:dyDescent="0.2">
       <c r="C91" s="2" t="s">
         <v>1196</v>
       </c>
     </row>
-    <row r="92" spans="2:4">
+    <row r="92" spans="2:4" x14ac:dyDescent="0.2">
       <c r="C92" s="2" t="s">
         <v>1200</v>
       </c>
     </row>
-    <row r="93" spans="2:4">
+    <row r="93" spans="2:4" x14ac:dyDescent="0.2">
       <c r="C93" s="2" t="s">
         <v>1195</v>
       </c>
@@ -24088,19 +24124,19 @@
         <v>1197</v>
       </c>
     </row>
-    <row r="94" spans="2:4">
+    <row r="94" spans="2:4" x14ac:dyDescent="0.2">
       <c r="C94" s="2" t="s">
         <v>1201</v>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="2" type="noConversion"/>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr published="0"/>
   <dimension ref="A1:R55"/>
   <sheetViews>
@@ -24108,9 +24144,9 @@
       <selection activeCell="R2" sqref="R2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:18">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>1169</v>
       </c>
@@ -24163,7 +24199,7 @@
         <v>1238</v>
       </c>
     </row>
-    <row r="2" spans="1:18">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -24216,7 +24252,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="3" spans="1:18">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>1</v>
       </c>
@@ -24269,7 +24305,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="4" spans="1:18">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>2</v>
       </c>
@@ -24322,7 +24358,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="5" spans="1:18">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>2</v>
       </c>
@@ -24375,7 +24411,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="6" spans="1:18">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>2</v>
       </c>
@@ -24428,7 +24464,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="7" spans="1:18">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>2</v>
       </c>
@@ -24481,7 +24517,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="8" spans="1:18">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>0</v>
       </c>
@@ -24534,7 +24570,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="9" spans="1:18">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>2</v>
       </c>
@@ -24587,7 +24623,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="10" spans="1:18">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>1</v>
       </c>
@@ -24640,7 +24676,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="11" spans="1:18">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>2</v>
       </c>
@@ -24693,7 +24729,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="12" spans="1:18">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>2</v>
       </c>
@@ -24746,7 +24782,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="13" spans="1:18">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>2</v>
       </c>
@@ -24799,7 +24835,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="14" spans="1:18">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>2</v>
       </c>
@@ -24852,7 +24888,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="15" spans="1:18" ht="12.75" customHeight="1">
+    <row r="15" spans="1:18" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>1</v>
       </c>
@@ -24905,7 +24941,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="16" spans="1:18">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>1</v>
       </c>
@@ -24958,7 +24994,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="17" spans="1:18">
+    <row r="17" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>1</v>
       </c>
@@ -25011,7 +25047,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="18" spans="1:18">
+    <row r="18" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>0</v>
       </c>
@@ -25064,7 +25100,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="19" spans="1:18">
+    <row r="19" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>1</v>
       </c>
@@ -25117,7 +25153,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="20" spans="1:18">
+    <row r="20" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>1</v>
       </c>
@@ -25170,7 +25206,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="21" spans="1:18">
+    <row r="21" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>0</v>
       </c>
@@ -25223,7 +25259,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="22" spans="1:18">
+    <row r="22" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>1</v>
       </c>
@@ -25276,7 +25312,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="23" spans="1:18">
+    <row r="23" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>2</v>
       </c>
@@ -25329,7 +25365,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="24" spans="1:18">
+    <row r="24" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>1</v>
       </c>
@@ -25382,7 +25418,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="25" spans="1:18">
+    <row r="25" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>0</v>
       </c>
@@ -25435,7 +25471,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="26" spans="1:18" ht="15" customHeight="1">
+    <row r="26" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="16">
         <v>0</v>
       </c>
@@ -25488,7 +25524,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="27" spans="1:18">
+    <row r="27" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>1</v>
       </c>
@@ -25541,7 +25577,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="28" spans="1:18">
+    <row r="28" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>0</v>
       </c>
@@ -25594,7 +25630,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="29" spans="1:18">
+    <row r="29" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>0</v>
       </c>
@@ -25647,7 +25683,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="30" spans="1:18">
+    <row r="30" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>2</v>
       </c>
@@ -25700,7 +25736,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="31" spans="1:18">
+    <row r="31" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>1</v>
       </c>
@@ -25753,7 +25789,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="32" spans="1:18">
+    <row r="32" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>1</v>
       </c>
@@ -25806,7 +25842,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="33" spans="1:18">
+    <row r="33" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>1</v>
       </c>
@@ -25859,7 +25895,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="34" spans="1:18">
+    <row r="34" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>2</v>
       </c>
@@ -25912,7 +25948,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="35" spans="1:18">
+    <row r="35" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>2</v>
       </c>
@@ -25965,7 +26001,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="36" spans="1:18">
+    <row r="36" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>1</v>
       </c>
@@ -26018,7 +26054,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="37" spans="1:18">
+    <row r="37" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>1</v>
       </c>
@@ -26071,7 +26107,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="38" spans="1:18">
+    <row r="38" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>2</v>
       </c>
@@ -26124,7 +26160,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="39" spans="1:18">
+    <row r="39" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>1</v>
       </c>
@@ -26177,7 +26213,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="40" spans="1:18">
+    <row r="40" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>2</v>
       </c>
@@ -26230,7 +26266,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="41" spans="1:18">
+    <row r="41" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A41">
         <v>1</v>
       </c>
@@ -26283,7 +26319,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="42" spans="1:18" s="22" customFormat="1" ht="15" customHeight="1">
+    <row r="42" spans="1:18" s="22" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="23">
         <v>2</v>
       </c>
@@ -26336,7 +26372,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="47" spans="1:18">
+    <row r="47" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A47">
         <v>7</v>
       </c>
@@ -26389,7 +26425,7 @@
         <v>1234</v>
       </c>
     </row>
-    <row r="48" spans="1:18">
+    <row r="48" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A48">
         <v>18</v>
       </c>
@@ -26442,7 +26478,7 @@
         <v>1235</v>
       </c>
     </row>
-    <row r="49" spans="1:17">
+    <row r="49" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A49">
         <v>16</v>
       </c>
@@ -26495,12 +26531,12 @@
         <v>1236</v>
       </c>
     </row>
-    <row r="50" spans="1:17">
+    <row r="50" spans="1:17" x14ac:dyDescent="0.2">
       <c r="Q50" t="s">
         <v>1237</v>
       </c>
     </row>
-    <row r="51" spans="1:17">
+    <row r="51" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A51">
         <f>SUM(A48:A49)</f>
         <v>34</v>
@@ -26562,21 +26598,21 @@
         <v>33</v>
       </c>
     </row>
-    <row r="53" spans="1:17">
+    <row r="53" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A53" s="2">
         <f>MIN(A51:O51)</f>
         <v>29</v>
       </c>
       <c r="B53" s="2"/>
     </row>
-    <row r="54" spans="1:17">
+    <row r="54" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A54" s="2">
         <f>MAX(A51:O51)</f>
         <v>41</v>
       </c>
       <c r="B54" s="2"/>
     </row>
-    <row r="55" spans="1:17">
+    <row r="55" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A55" s="2">
         <f>AVERAGE(A51:O51)</f>
         <v>36.93333333333333</v>
@@ -26590,7 +26626,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr published="0"/>
   <dimension ref="A1:DP1"/>
   <sheetViews>
@@ -26598,9 +26634,9 @@
       <selection activeCell="D1" sqref="D1:H1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:120">
+    <row r="1" spans="1:120" x14ac:dyDescent="0.2">
       <c r="A1">
         <v>68.014414634146334</v>
       </c>

</xml_diff>